<commit_message>
:pencil2: make better example data
</commit_message>
<xml_diff>
--- a/public/static/excels/giang-vien-example.xlsx
+++ b/public/static/excels/giang-vien-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\projects\b4e_new\school\frontend\public\static\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangNam\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62607C46-107A-4012-B810-D8DFD7A0FE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81291C40-3D15-4BA1-8E75-C1E7366E4C9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{04DDEBD4-CB3A-4746-B62E-0BCB03B1A5A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2308C60D-495E-4A7C-8117-8DAC76F24E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
+    <t>Mã giáo vụ</t>
+  </si>
+  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -57,7 +60,7 @@
     <t>Viện CNTT&amp;TT</t>
   </si>
   <si>
-    <t>A0X+4i2FyudeVsKB6NLv8uLoGTcfBGEczZucKNwJdSMF</t>
+    <t>31d0e835390695f825a1322b38bdb3de71c075...</t>
   </si>
   <si>
     <t>Lý Thị C</t>
@@ -69,7 +72,7 @@
     <t>Viện Sư phạm Kỹ thuật</t>
   </si>
   <si>
-    <t>AnLpO4jxLPGUjNBpJmnOja/FpXdncPS363uMJwYnS0n9</t>
+    <t>81741c77ad5e5ff27ec91a94ced51b82a37968...</t>
   </si>
   <si>
     <t>Lê Thị D</t>
@@ -81,7 +84,7 @@
     <t>Viện Ngoại ngữ</t>
   </si>
   <si>
-    <t>Aq7DZm5J4jBJNPMCSaEAg2qOY9icCYoigIBOLAN8WPiV</t>
+    <t>ecfdc8f69b08d0260ba2309d7b8e064a28f0eb5...</t>
   </si>
   <si>
     <t>Trần Văn E</t>
@@ -93,7 +96,7 @@
     <t>Viện Điện tử viễn thông</t>
   </si>
   <si>
-    <t>AxrZLzzkIheuNY3Ff0VawaXdVAdjlGq61bUAocL/ZXgG</t>
+    <t>4d4ebfbf5ea1f3b61b04434528844956ab6890536...</t>
   </si>
   <si>
     <t>Đào Thị F</t>
@@ -105,25 +108,22 @@
     <t>Viện Điều khiển Tự động hóa</t>
   </si>
   <si>
-    <t>A22V6uhd9uFISY7IcQshKuJ5sEBMuoORHqsTYL5gHQav</t>
-  </si>
-  <si>
-    <t>Mã giảng viên</t>
-  </si>
-  <si>
-    <t>Gv1234</t>
-  </si>
-  <si>
-    <t>Gv1235</t>
-  </si>
-  <si>
-    <t>Gv1236</t>
-  </si>
-  <si>
-    <t>Gv1237</t>
-  </si>
-  <si>
-    <t>Gv1238</t>
+    <t>4d4ebfbf5ea1f3b61b04434528844956ab6890...</t>
+  </si>
+  <si>
+    <t>GV1234</t>
+  </si>
+  <si>
+    <t>GV1235</t>
+  </si>
+  <si>
+    <t>GV1236</t>
+  </si>
+  <si>
+    <t>GV1237</t>
+  </si>
+  <si>
+    <t>GV1238</t>
   </si>
 </sst>
 </file>
@@ -474,38 +474,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A889D353-129A-4ACB-8F59-FBB358968A12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C6C5F7-0189-4E4D-AD28-B6761338D5B8}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -513,16 +512,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -530,16 +529,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -547,16 +546,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -564,16 +563,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -581,19 +580,20 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:pencil2: update data-example to 32byte pubkey
</commit_message>
<xml_diff>
--- a/public/static/excels/giang-vien-example.xlsx
+++ b/public/static/excels/giang-vien-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangNam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\projects\b4e_new\school\frontend\public\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81291C40-3D15-4BA1-8E75-C1E7366E4C9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F84E32-F1D5-420E-AAC9-F73CBA32C7D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2308C60D-495E-4A7C-8117-8DAC76F24E57}"/>
+    <workbookView xWindow="-28920" yWindow="-1245" windowWidth="29040" windowHeight="15990" xr2:uid="{2308C60D-495E-4A7C-8117-8DAC76F24E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t>Mã giáo vụ</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Viện CNTT&amp;TT</t>
   </si>
   <si>
-    <t>31d0e835390695f825a1322b38bdb3de71c075...</t>
-  </si>
-  <si>
     <t>Lý Thị C</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Viện Sư phạm Kỹ thuật</t>
   </si>
   <si>
-    <t>81741c77ad5e5ff27ec91a94ced51b82a37968...</t>
-  </si>
-  <si>
     <t>Lê Thị D</t>
   </si>
   <si>
@@ -84,9 +75,6 @@
     <t>Viện Ngoại ngữ</t>
   </si>
   <si>
-    <t>ecfdc8f69b08d0260ba2309d7b8e064a28f0eb5...</t>
-  </si>
-  <si>
     <t>Trần Văn E</t>
   </si>
   <si>
@@ -96,9 +84,6 @@
     <t>Viện Điện tử viễn thông</t>
   </si>
   <si>
-    <t>4d4ebfbf5ea1f3b61b04434528844956ab6890536...</t>
-  </si>
-  <si>
     <t>Đào Thị F</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
     <t>Viện Điều khiển Tự động hóa</t>
   </si>
   <si>
-    <t>4d4ebfbf5ea1f3b61b04434528844956ab6890...</t>
-  </si>
-  <si>
     <t>GV1234</t>
   </si>
   <si>
@@ -124,6 +106,24 @@
   </si>
   <si>
     <t>GV1238</t>
+  </si>
+  <si>
+    <t>Mã giảng viên</t>
+  </si>
+  <si>
+    <t>02a2e3f2b6b9ec1155979ee691072bd17fc9facd0d7751417fdf4d7af760ce962a</t>
+  </si>
+  <si>
+    <t>02992cf23456bf4167fc2d69f70ee36361af8ad2a2512f9a660be320086211f3e0</t>
+  </si>
+  <si>
+    <t>028b921e7d9e7e0ece5660dc48e6c7b84d8c547a3f3d42990e67897858968120d5</t>
+  </si>
+  <si>
+    <t>02a09d011afd12783ab87f44ad1932dcca1f59e13ba904d2c7b465df31df681a32</t>
+  </si>
+  <si>
+    <t>0351befccfa9fa6ba05d16a2eb94a593f773f7e9db0138ba831424905174d730fe</t>
   </si>
 </sst>
 </file>
@@ -478,118 +478,118 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>